<commit_message>
added final seoul, overseas, and third survey
</commit_message>
<xml_diff>
--- a/data/2021_민주당 경선결과.xlsx
+++ b/data/2021_민주당 경선결과.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="42">
   <si>
     <t>권리당원</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,6 +182,10 @@
   </si>
   <si>
     <t>(9월11일 기준)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재외국민</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -939,7 +944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -949,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.45"/>
@@ -3034,29 +3039,53 @@
       <c r="B27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="C27" s="9">
+        <v>44100</v>
+      </c>
+      <c r="D27" s="5">
+        <v>31320</v>
+      </c>
+      <c r="E27" s="5">
+        <v>1746</v>
+      </c>
+      <c r="F27" s="5">
+        <v>8687</v>
+      </c>
       <c r="G27" s="45">
         <f>SUM(C27,D27,E27,F27)</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+        <v>85853</v>
+      </c>
+      <c r="H27" s="9">
+        <v>1617</v>
+      </c>
+      <c r="I27" s="5">
+        <v>1101</v>
+      </c>
+      <c r="J27" s="5">
+        <v>152</v>
+      </c>
+      <c r="K27" s="5">
+        <v>125</v>
+      </c>
       <c r="L27" s="45">
         <f>SUM(H27,I27,J27,K27)</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="9"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
+        <v>2995</v>
+      </c>
+      <c r="M27" s="9">
+        <v>20</v>
+      </c>
+      <c r="N27" s="5">
+        <v>24</v>
+      </c>
+      <c r="O27" s="5">
+        <v>0</v>
+      </c>
+      <c r="P27" s="5">
+        <v>1</v>
+      </c>
       <c r="Q27" s="45">
         <f>SUM(M27,N27,O27,P27)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="R27" s="7"/>
       <c r="S27" s="4"/>
@@ -3065,25 +3094,27 @@
       <c r="V27" s="8"/>
       <c r="W27" s="9">
         <f>SUM(C27,H27,M27)</f>
-        <v>0</v>
+        <v>45737</v>
       </c>
       <c r="X27" s="5">
         <f>SUM(D27,I27,N27)</f>
-        <v>0</v>
+        <v>32445</v>
       </c>
       <c r="Y27" s="5">
         <f>SUM(E27,J27,O27)</f>
-        <v>0</v>
+        <v>1898</v>
       </c>
       <c r="Z27" s="5">
         <f>SUM(F27,K27,P27)</f>
-        <v>0</v>
+        <v>8813</v>
       </c>
       <c r="AA27" s="47">
         <f>SUM(W27,X27,Y27,Z27)</f>
-        <v>0</v>
-      </c>
-      <c r="AB27" s="10"/>
+        <v>88893</v>
+      </c>
+      <c r="AB27" s="10">
+        <v>144481</v>
+      </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A28" s="14" t="s">
@@ -3092,55 +3123,55 @@
       <c r="B28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="35" t="e">
+      <c r="C28" s="35">
         <f>C27/G27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D28" s="36" t="e">
+        <v>51.366871279978568</v>
+      </c>
+      <c r="D28" s="36">
         <f>D27/G27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="36" t="e">
+        <v>36.480961643739882</v>
+      </c>
+      <c r="E28" s="36">
         <f>E27/G27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="36" t="e">
+        <v>2.0337087812889476</v>
+      </c>
+      <c r="F28" s="36">
         <f>F27/G27*100</f>
-        <v>#DIV/0!</v>
+        <v>10.118458294992603</v>
       </c>
       <c r="G28" s="37"/>
-      <c r="H28" s="35" t="e">
+      <c r="H28" s="35">
         <f>H27/L27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" s="36" t="e">
+        <v>53.989983305509185</v>
+      </c>
+      <c r="I28" s="36">
         <f>I27/L27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J28" s="36" t="e">
+        <v>36.761268781302171</v>
+      </c>
+      <c r="J28" s="36">
         <f>J27/L27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K28" s="36" t="e">
+        <v>5.0751252086811354</v>
+      </c>
+      <c r="K28" s="36">
         <f>K27/L27*100</f>
-        <v>#DIV/0!</v>
+        <v>4.1736227045075127</v>
       </c>
       <c r="L28" s="37"/>
-      <c r="M28" s="35" t="e">
+      <c r="M28" s="35">
         <f>M27/Q27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N28" s="36" t="e">
+        <v>44.444444444444443</v>
+      </c>
+      <c r="N28" s="36">
         <f t="shared" ref="N28" si="42">N27/Q27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="36" t="e">
+        <v>53.333333333333336</v>
+      </c>
+      <c r="O28" s="36">
         <f t="shared" ref="O28" si="43">O27/Q27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="36" t="e">
+        <v>0</v>
+      </c>
+      <c r="P28" s="36">
         <f t="shared" ref="P28" si="44">P27/Q27*100</f>
-        <v>#DIV/0!</v>
+        <v>2.2222222222222223</v>
       </c>
       <c r="Q28" s="37"/>
       <c r="R28" s="7"/>
@@ -3148,25 +3179,25 @@
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="8"/>
-      <c r="W28" s="35" t="e">
+      <c r="W28" s="35">
         <f>W27/AA27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X28" s="36" t="e">
+        <v>51.451745356777245</v>
+      </c>
+      <c r="X28" s="36">
         <f t="shared" ref="X28" si="45">X27/AA27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y28" s="36" t="e">
+        <v>36.498936924167261</v>
+      </c>
+      <c r="Y28" s="36">
         <f t="shared" ref="Y28" si="46">Y27/AA27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z28" s="36" t="e">
+        <v>2.1351512492547222</v>
+      </c>
+      <c r="Z28" s="36">
         <f t="shared" ref="Z28" si="47">Z27/AA27*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA28" s="36" t="e">
+        <v>9.9141664698007705</v>
+      </c>
+      <c r="AA28" s="36">
         <f t="shared" ref="AA28" si="48">AA27/AB27*100</f>
-        <v>#DIV/0!</v>
+        <v>61.525736948110819</v>
       </c>
       <c r="AB28" s="12"/>
     </row>
@@ -3192,35 +3223,45 @@
       <c r="O29" s="5"/>
       <c r="P29" s="5"/>
       <c r="Q29" s="10"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
+      <c r="R29" s="9">
+        <v>70441</v>
+      </c>
+      <c r="S29" s="5">
+        <v>155220</v>
+      </c>
+      <c r="T29" s="5">
+        <v>2784</v>
+      </c>
+      <c r="U29" s="5">
+        <v>20435</v>
+      </c>
       <c r="V29" s="10">
         <f>SUM(R29,S29,T29,U29)</f>
-        <v>0</v>
+        <v>248880</v>
       </c>
       <c r="W29" s="9">
         <f>R29</f>
-        <v>0</v>
+        <v>70441</v>
       </c>
       <c r="X29" s="5">
         <f>S29</f>
-        <v>0</v>
+        <v>155220</v>
       </c>
       <c r="Y29" s="5">
         <f>T29</f>
-        <v>0</v>
+        <v>2784</v>
       </c>
       <c r="Z29" s="5">
         <f>U29</f>
-        <v>0</v>
+        <v>20435</v>
       </c>
       <c r="AA29" s="5">
         <f>V29</f>
-        <v>0</v>
-      </c>
-      <c r="AB29" s="10"/>
+        <v>248880</v>
+      </c>
+      <c r="AB29" s="10">
+        <v>305779</v>
+      </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
@@ -3244,42 +3285,42 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="12"/>
-      <c r="R30" s="35" t="e">
+      <c r="R30" s="35">
         <f>R29/V29*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S30" s="36" t="e">
+        <v>28.30319832851173</v>
+      </c>
+      <c r="S30" s="36">
         <f>S29/V29*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T30" s="36" t="e">
+        <v>62.367405978784952</v>
+      </c>
+      <c r="T30" s="36">
         <f>T29/V29*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U30" s="36" t="e">
+        <v>1.1186113789778205</v>
+      </c>
+      <c r="U30" s="36">
         <f>U29/V29*100</f>
-        <v>#DIV/0!</v>
+        <v>8.2107843137254903</v>
       </c>
       <c r="V30" s="37"/>
-      <c r="W30" s="35" t="e">
+      <c r="W30" s="35">
         <f>R30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X30" s="36" t="e">
+        <v>28.30319832851173</v>
+      </c>
+      <c r="X30" s="36">
         <f>S30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y30" s="36" t="e">
+        <v>62.367405978784952</v>
+      </c>
+      <c r="Y30" s="36">
         <f>T30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z30" s="36" t="e">
+        <v>1.1186113789778205</v>
+      </c>
+      <c r="Z30" s="36">
         <f>U30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA30" s="36" t="e">
+        <v>8.2107843137254903</v>
+      </c>
+      <c r="AA30" s="36">
         <f>AA29/AB29*100</f>
-        <v>#DIV/0!</v>
+        <v>81.392116528603992</v>
       </c>
       <c r="AB30" s="12"/>
     </row>
@@ -3292,51 +3333,51 @@
       </c>
       <c r="C31" s="39">
         <f>SUM(C3,C5,C7,C9,C13,C15,C17,C19,C21,C25,C27)</f>
-        <v>170827</v>
+        <v>214927</v>
       </c>
       <c r="D31" s="40">
         <f t="shared" ref="D31:G31" si="49">SUM(D3,D5,D7,D9,D13,D15,D17,D19,D21,D25,D27)</f>
-        <v>111298</v>
+        <v>142618</v>
       </c>
       <c r="E31" s="40">
         <f t="shared" si="49"/>
-        <v>4180</v>
+        <v>5926</v>
       </c>
       <c r="F31" s="40">
         <f t="shared" si="49"/>
-        <v>23596</v>
+        <v>32283</v>
       </c>
       <c r="G31" s="41">
         <f t="shared" si="49"/>
-        <v>309901</v>
+        <v>395754</v>
       </c>
       <c r="H31" s="39">
         <f t="shared" ref="H31:Q31" si="50">SUM(H3,H5,H7,H9,H13,H15,H17,H19,H21,H25,H27)</f>
-        <v>5467</v>
+        <v>7084</v>
       </c>
       <c r="I31" s="40">
         <f t="shared" si="50"/>
-        <v>3610</v>
+        <v>4711</v>
       </c>
       <c r="J31" s="40">
         <f t="shared" si="50"/>
-        <v>143</v>
+        <v>295</v>
       </c>
       <c r="K31" s="40">
         <f t="shared" si="50"/>
-        <v>433</v>
+        <v>558</v>
       </c>
       <c r="L31" s="41">
         <f t="shared" si="50"/>
-        <v>9653</v>
+        <v>12648</v>
       </c>
       <c r="M31" s="39">
         <f t="shared" si="50"/>
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="N31" s="40">
         <f t="shared" si="50"/>
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="O31" s="40">
         <f t="shared" si="50"/>
@@ -3344,55 +3385,55 @@
       </c>
       <c r="P31" s="40">
         <f t="shared" si="50"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q31" s="41">
         <f t="shared" si="50"/>
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="R31" s="39">
         <f>SUM(R11,R23,R29)</f>
-        <v>425999</v>
+        <v>496440</v>
       </c>
       <c r="S31" s="40">
         <f t="shared" ref="S31:U31" si="51">SUM(S11,S23,S29)</f>
-        <v>255343</v>
+        <v>410563</v>
       </c>
       <c r="T31" s="40">
         <f t="shared" si="51"/>
-        <v>13247</v>
+        <v>16031</v>
       </c>
       <c r="U31" s="40">
         <f t="shared" si="51"/>
-        <v>75209</v>
+        <v>95644</v>
       </c>
       <c r="V31" s="41">
         <f>SUM(V11,V23,V29)</f>
-        <v>769798</v>
+        <v>1018678</v>
       </c>
       <c r="W31" s="39">
         <f>SUM(W3,W5,W7,W9,W11,W13,W15,W17,W19,W21,W23,W25,W27,W29)</f>
-        <v>602357</v>
+        <v>718535</v>
       </c>
       <c r="X31" s="40">
         <f t="shared" ref="X31:AB31" si="52">SUM(X3,X5,X7,X9,X11,X13,X15,X17,X19,X21,X23,X25,X27,X29)</f>
-        <v>370324</v>
+        <v>557989</v>
       </c>
       <c r="Y31" s="40">
         <f t="shared" si="52"/>
-        <v>17570</v>
+        <v>22252</v>
       </c>
       <c r="Z31" s="40">
         <f t="shared" si="52"/>
-        <v>99246</v>
+        <v>128494</v>
       </c>
       <c r="AA31" s="40">
         <f t="shared" si="52"/>
-        <v>1089497</v>
+        <v>1427270</v>
       </c>
       <c r="AB31" s="41">
         <f t="shared" si="52"/>
-        <v>1714321</v>
+        <v>2164581</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -3404,45 +3445,45 @@
       </c>
       <c r="C32" s="42">
         <f>C31/G31*100</f>
-        <v>55.123087695747998</v>
+        <v>54.308231881421285</v>
       </c>
       <c r="D32" s="43">
         <f>D31/G31*100</f>
-        <v>35.914049970797123</v>
+        <v>36.037033106424701</v>
       </c>
       <c r="E32" s="43">
         <f>E31/G31*100</f>
-        <v>1.3488178482805799</v>
+        <v>1.4973948462934044</v>
       </c>
       <c r="F32" s="43">
         <f>F31/G31*100</f>
-        <v>7.614044485174297</v>
+        <v>8.1573401658606102</v>
       </c>
       <c r="G32" s="44"/>
       <c r="H32" s="43">
         <f>H31/L31*100</f>
-        <v>56.635242929659171</v>
+        <v>56.008855154965211</v>
       </c>
       <c r="I32" s="43">
         <f>I31/L31*100</f>
-        <v>37.397700196830002</v>
+        <v>37.24699557242252</v>
       </c>
       <c r="J32" s="43">
         <f>J31/L31*100</f>
-        <v>1.4814047446389724</v>
+        <v>2.3323845667299179</v>
       </c>
       <c r="K32" s="43">
         <f>K31/L31*100</f>
-        <v>4.4856521288718536</v>
+        <v>4.4117647058823533</v>
       </c>
       <c r="L32" s="43"/>
       <c r="M32" s="42">
         <f>M31/Q31*100</f>
-        <v>44.137931034482762</v>
+        <v>44.210526315789473</v>
       </c>
       <c r="N32" s="43">
         <f>N31/Q31*100</f>
-        <v>50.344827586206897</v>
+        <v>51.05263157894737</v>
       </c>
       <c r="O32" s="43">
         <f>O31/Q31*100</f>
@@ -3450,45 +3491,45 @@
       </c>
       <c r="P32" s="43">
         <f>P31/Q31*100</f>
-        <v>5.5172413793103452</v>
+        <v>4.7368421052631584</v>
       </c>
       <c r="Q32" s="44"/>
       <c r="R32" s="42">
         <f>R31/V31*100</f>
-        <v>55.33906297496226</v>
+        <v>48.733750998843597</v>
       </c>
       <c r="S32" s="43">
         <f>S31/V31*100</f>
-        <v>33.170130345882946</v>
+        <v>40.303511021147017</v>
       </c>
       <c r="T32" s="43">
         <f>T31/V31*100</f>
-        <v>1.7208410518083965</v>
+        <v>1.5737063134768789</v>
       </c>
       <c r="U32" s="43">
         <f>U31/V31*100</f>
-        <v>9.7699656273463944</v>
+        <v>9.3890316665325066</v>
       </c>
       <c r="V32" s="44"/>
       <c r="W32" s="42">
         <f>W31/AA31*100</f>
-        <v>55.287623554722963</v>
+        <v>50.343312757922462</v>
       </c>
       <c r="X32" s="43">
         <f>X31/AA31*100</f>
-        <v>33.990364360801365</v>
+        <v>39.094845404163195</v>
       </c>
       <c r="Y32" s="43">
         <f>Y31/AA31*100</f>
-        <v>1.612670801296378</v>
+        <v>1.5590603039368867</v>
       </c>
       <c r="Z32" s="43">
         <f>Z31/AA31*100</f>
-        <v>9.1093412831793028</v>
+        <v>9.0027815339774531</v>
       </c>
       <c r="AA32" s="43">
         <f>AA31/AB31*100</f>
-        <v>63.552683540597123</v>
+        <v>65.937472425379312</v>
       </c>
       <c r="AB32" s="49"/>
     </row>
@@ -3504,4 +3545,99 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="33" orientation="landscape" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="5" width="7.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3"/>
+      <c r="B1" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+    </row>
+    <row r="2" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1370</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2403</v>
+      </c>
+      <c r="D3" s="5">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5">
+        <v>541</v>
+      </c>
+      <c r="F3" s="10">
+        <f>SUM(B3,C3,D3,E3)</f>
+        <v>4323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="35">
+        <f>B3/F3*100</f>
+        <v>31.690955355077495</v>
+      </c>
+      <c r="C4" s="36">
+        <f>C3/F3*100</f>
+        <v>55.586398334489942</v>
+      </c>
+      <c r="D4" s="36">
+        <f>D3/F3*100</f>
+        <v>0.20818875780707841</v>
+      </c>
+      <c r="E4" s="36">
+        <f>E3/F3*100</f>
+        <v>12.51445755262549</v>
+      </c>
+      <c r="F4" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>